<commit_message>
Code changes in Screen Orientation and Utility File
</commit_message>
<xml_diff>
--- a/src/datasheet/Ebay.xlsx
+++ b/src/datasheet/Ebay.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="714" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="714" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="184">
   <si>
     <t>Project Name</t>
   </si>
@@ -48,7 +48,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Summary of the all test case execution </t>
+    <t>Summary of the all test case execution</t>
   </si>
   <si>
     <t>Tested Device</t>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>Failed</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>TC003</t>
   </si>
   <si>
     <t>Total Scenarios Covered</t>
@@ -1117,8 +1126,8 @@
   </sheetPr>
   <dimension ref="A1:J65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1282,8 +1291,8 @@
       <c r="J8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="n">
-        <v>1.1</v>
+      <c r="A9" s="15" t="s">
+        <v>24</v>
       </c>
       <c r="B9" s="16" t="str">
         <f aca="false">TC001!B4</f>
@@ -1308,8 +1317,8 @@
       <c r="J9" s="18"/>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="n">
-        <v>1.2</v>
+      <c r="A10" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="B10" s="16" t="str">
         <f aca="false">TC002!B4</f>
@@ -1336,8 +1345,8 @@
       <c r="J10" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="n">
-        <v>1.3</v>
+      <c r="A11" s="15" t="s">
+        <v>26</v>
       </c>
       <c r="B11" s="16" t="str">
         <f aca="false">TC003!B4</f>
@@ -1369,11 +1378,11 @@
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
       <c r="G12" s="20" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H12" s="21" t="n">
-        <f aca="false">COUNTA(A9:A10)</f>
-        <v>2</v>
+        <f aca="false">COUNTA(A9:A11)</f>
+        <v>3</v>
       </c>
       <c r="I12" s="21"/>
       <c r="J12" s="22"/>
@@ -1386,11 +1395,11 @@
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="20" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H13" s="21" t="n">
-        <f aca="false">SUM(G9:G10)</f>
-        <v>46</v>
+        <f aca="false">SUM(G9:G11)</f>
+        <v>53</v>
       </c>
       <c r="I13" s="21"/>
       <c r="J13" s="22"/>
@@ -1403,16 +1412,16 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H14" s="21" t="n">
-        <f aca="false">SUM(H9:H10)</f>
+        <f aca="false">SUM(H9:H11)</f>
         <v>0</v>
       </c>
       <c r="I14" s="21"/>
       <c r="J14" s="22"/>
     </row>
-    <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="19"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
@@ -1420,15 +1429,16 @@
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
       <c r="G15" s="20" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H15" s="21" t="n">
-        <f aca="false">SUM(I9:I10)</f>
+        <f aca="false">SUM(I9:I11)</f>
         <v>0</v>
       </c>
       <c r="I15" s="21"/>
       <c r="J15" s="23"/>
     </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1492,226 +1502,226 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="26" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="26" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="26" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="26" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="26" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="26" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="26" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="26" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="26" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="26" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="26" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="26" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="26" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="26" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="26" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="26" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="26" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="26" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="26" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1833,7 +1843,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -1851,7 +1861,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -1866,10 +1876,10 @@
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -1884,10 +1894,10 @@
     </row>
     <row r="5" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="34" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
@@ -1920,31 +1930,31 @@
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="J7" s="30"/>
     </row>
@@ -1953,18 +1963,18 @@
         <v>1</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C8" s="37"/>
       <c r="D8" s="38" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E8" s="39"/>
       <c r="F8" s="40" t="n">
         <v>10</v>
       </c>
       <c r="G8" s="41" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H8" s="42"/>
       <c r="I8" s="43"/>
@@ -1975,15 +1985,15 @@
         <v>2</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C9" s="37"/>
       <c r="D9" s="38" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E9" s="39"/>
       <c r="F9" s="44" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G9" s="45"/>
       <c r="H9" s="42"/>
@@ -1995,15 +2005,15 @@
         <v>3</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="38" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E10" s="39"/>
       <c r="F10" s="44" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G10" s="45"/>
       <c r="H10" s="42"/>
@@ -2016,15 +2026,15 @@
         <v>4</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C11" s="37"/>
       <c r="D11" s="38" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E11" s="39"/>
       <c r="F11" s="44" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G11" s="45"/>
       <c r="H11" s="42"/>
@@ -2037,15 +2047,15 @@
         <v>5</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C12" s="37"/>
       <c r="D12" s="38" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E12" s="39"/>
       <c r="F12" s="44" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G12" s="45"/>
       <c r="H12" s="42"/>
@@ -2058,15 +2068,15 @@
         <v>6</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C13" s="37"/>
       <c r="D13" s="16" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="46" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G13" s="47"/>
       <c r="H13" s="48"/>
@@ -2079,15 +2089,15 @@
         <v>7</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="38" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="46" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G14" s="47"/>
       <c r="H14" s="48"/>
@@ -2100,15 +2110,15 @@
         <v>8</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C15" s="37"/>
       <c r="D15" s="38" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="46" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G15" s="47"/>
       <c r="H15" s="48"/>
@@ -2121,15 +2131,15 @@
         <v>9</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C16" s="37"/>
       <c r="D16" s="16" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="37" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G16" s="47"/>
       <c r="H16" s="48"/>
@@ -2142,15 +2152,15 @@
         <v>10</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="38" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="44" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G17" s="47"/>
       <c r="H17" s="48"/>
@@ -2163,15 +2173,15 @@
         <v>11</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C18" s="37"/>
       <c r="D18" s="38" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E18" s="16"/>
       <c r="F18" s="37" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G18" s="47"/>
       <c r="H18" s="48"/>
@@ -2204,7 +2214,7 @@
       <c r="F20" s="49"/>
       <c r="G20" s="49"/>
       <c r="H20" s="50" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="I20" s="51" t="n">
         <f aca="false">COUNTIF(I8:I18,"Pass")</f>
@@ -2221,7 +2231,7 @@
       <c r="F21" s="49"/>
       <c r="G21" s="49"/>
       <c r="H21" s="50" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="I21" s="52" t="n">
         <f aca="false">COUNTIF(I8:I18,"Fail")</f>
@@ -2300,7 +2310,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -2318,7 +2328,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -2333,10 +2343,10 @@
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -2351,10 +2361,10 @@
     </row>
     <row r="5" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="34" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
@@ -2385,31 +2395,31 @@
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="J7" s="30"/>
     </row>
@@ -2418,18 +2428,18 @@
         <v>1</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C8" s="37"/>
       <c r="D8" s="38" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F8" s="37"/>
       <c r="G8" s="47" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H8" s="48"/>
       <c r="I8" s="43"/>
@@ -2440,14 +2450,14 @@
         <v>2</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C9" s="37"/>
       <c r="D9" s="38" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F9" s="37"/>
       <c r="G9" s="47"/>
@@ -2460,17 +2470,17 @@
         <v>3</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="38" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="G10" s="47"/>
       <c r="H10" s="48"/>
@@ -2482,14 +2492,14 @@
         <v>4</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C11" s="37"/>
       <c r="D11" s="38" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F11" s="37"/>
       <c r="G11" s="47"/>
@@ -2502,18 +2512,18 @@
         <v>5</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C12" s="37"/>
       <c r="D12" s="38" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F12" s="37"/>
       <c r="G12" s="47" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H12" s="48"/>
       <c r="I12" s="43"/>
@@ -2524,18 +2534,18 @@
         <v>6</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C13" s="37"/>
       <c r="D13" s="38" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E13" s="39"/>
       <c r="F13" s="40" t="n">
         <v>1</v>
       </c>
       <c r="G13" s="41" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H13" s="48"/>
       <c r="I13" s="43"/>
@@ -2546,15 +2556,15 @@
         <v>7</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="38" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E14" s="26"/>
       <c r="F14" s="37" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="G14" s="47"/>
       <c r="H14" s="48"/>
@@ -2566,11 +2576,11 @@
         <v>8</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C15" s="37"/>
       <c r="D15" s="38" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E15" s="26"/>
       <c r="F15" s="37" t="n">
@@ -2586,14 +2596,14 @@
         <v>9</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C16" s="37"/>
       <c r="D16" s="38" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E16" s="53" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F16" s="37"/>
       <c r="G16" s="47"/>
@@ -2606,14 +2616,14 @@
         <v>10</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="38" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F17" s="37"/>
       <c r="G17" s="47"/>
@@ -2626,18 +2636,18 @@
         <v>11</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C18" s="37"/>
       <c r="D18" s="38" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E18" s="39"/>
       <c r="F18" s="40" t="n">
         <v>1</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H18" s="48"/>
       <c r="I18" s="43"/>
@@ -2648,15 +2658,15 @@
         <v>12</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C19" s="37"/>
       <c r="D19" s="38" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="37" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G19" s="47"/>
       <c r="H19" s="48"/>
@@ -2668,18 +2678,18 @@
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C20" s="37"/>
       <c r="D20" s="38" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F20" s="37"/>
       <c r="G20" s="47" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H20" s="48"/>
       <c r="I20" s="43"/>
@@ -2690,18 +2700,18 @@
         <v>14</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C21" s="37"/>
       <c r="D21" s="38" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F21" s="37"/>
       <c r="G21" s="47" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H21" s="48"/>
       <c r="I21" s="43"/>
@@ -2712,11 +2722,11 @@
         <v>15</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C22" s="37"/>
       <c r="D22" s="38" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E22" s="26"/>
       <c r="F22" s="37"/>
@@ -2730,11 +2740,11 @@
         <v>16</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C23" s="37"/>
       <c r="D23" s="38" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E23" s="26"/>
       <c r="F23" s="37"/>
@@ -2748,11 +2758,11 @@
         <v>17</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C24" s="37"/>
       <c r="D24" s="38" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E24" s="26"/>
       <c r="F24" s="37"/>
@@ -2766,18 +2776,18 @@
         <v>18</v>
       </c>
       <c r="B25" s="38" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C25" s="37"/>
       <c r="D25" s="38" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E25" s="39"/>
       <c r="F25" s="40" t="n">
         <v>1</v>
       </c>
       <c r="G25" s="41" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H25" s="48"/>
       <c r="I25" s="43"/>
@@ -2788,18 +2798,18 @@
         <v>19</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C26" s="37"/>
       <c r="D26" s="38" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E26" s="53"/>
       <c r="F26" s="37" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="G26" s="47" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H26" s="48"/>
       <c r="I26" s="43"/>
@@ -2810,18 +2820,18 @@
         <v>20</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C27" s="37"/>
       <c r="D27" s="38" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F27" s="37"/>
       <c r="G27" s="47" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H27" s="48"/>
       <c r="I27" s="43"/>
@@ -2832,14 +2842,14 @@
         <v>21</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C28" s="37"/>
       <c r="D28" s="38" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F28" s="37"/>
       <c r="G28" s="47"/>
@@ -2852,14 +2862,14 @@
         <v>22</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C29" s="37"/>
       <c r="D29" s="38" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F29" s="37"/>
       <c r="G29" s="47"/>
@@ -2872,14 +2882,14 @@
         <v>23</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C30" s="37"/>
       <c r="D30" s="38" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F30" s="37"/>
       <c r="G30" s="47"/>
@@ -2892,14 +2902,14 @@
         <v>24</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C31" s="37"/>
       <c r="D31" s="38" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E31" s="54" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F31" s="37"/>
       <c r="G31" s="47"/>
@@ -2912,17 +2922,17 @@
         <v>25</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C32" s="37"/>
       <c r="D32" s="38" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F32" s="47" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G32" s="47"/>
       <c r="H32" s="48"/>
@@ -2934,17 +2944,17 @@
         <v>26</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C33" s="37"/>
       <c r="D33" s="38" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E33" s="54" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F33" s="37" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G33" s="47"/>
       <c r="H33" s="48"/>
@@ -2956,14 +2966,14 @@
         <v>27</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C34" s="37"/>
       <c r="D34" s="38" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F34" s="37"/>
       <c r="G34" s="47"/>
@@ -2976,18 +2986,18 @@
         <v>28</v>
       </c>
       <c r="B35" s="38" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C35" s="37"/>
       <c r="D35" s="38" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E35" s="39"/>
       <c r="F35" s="40" t="n">
         <v>1</v>
       </c>
       <c r="G35" s="41" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H35" s="48"/>
       <c r="I35" s="43"/>
@@ -2998,15 +3008,15 @@
         <v>29</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C36" s="37"/>
       <c r="D36" s="38" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E36" s="26"/>
       <c r="F36" s="37" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="G36" s="47"/>
       <c r="H36" s="48"/>
@@ -3018,14 +3028,14 @@
         <v>30</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C37" s="37"/>
       <c r="D37" s="38" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F37" s="37"/>
       <c r="G37" s="47"/>
@@ -3038,18 +3048,18 @@
         <v>31</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C38" s="37"/>
       <c r="D38" s="38" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E38" s="39"/>
       <c r="F38" s="40" t="n">
         <v>1</v>
       </c>
       <c r="G38" s="41" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H38" s="48"/>
       <c r="I38" s="43"/>
@@ -3060,15 +3070,15 @@
         <v>32</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C39" s="37"/>
       <c r="D39" s="38" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E39" s="26"/>
       <c r="F39" s="37" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="G39" s="47"/>
       <c r="H39" s="48"/>
@@ -3080,17 +3090,17 @@
         <v>33</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C40" s="37"/>
       <c r="D40" s="38" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F40" s="37" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="G40" s="47"/>
       <c r="H40" s="48"/>
@@ -3102,14 +3112,14 @@
         <v>34</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C41" s="37"/>
       <c r="D41" s="38" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F41" s="37"/>
       <c r="G41" s="47"/>
@@ -3122,14 +3132,14 @@
         <v>35</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C42" s="37"/>
       <c r="D42" s="38" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E42" s="54" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F42" s="37"/>
       <c r="G42" s="47"/>
@@ -3163,7 +3173,7 @@
       <c r="F44" s="49"/>
       <c r="G44" s="49"/>
       <c r="H44" s="50" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="I44" s="51" t="n">
         <f aca="false">COUNTIF(I8:I42,"Pass")</f>
@@ -3180,7 +3190,7 @@
       <c r="F45" s="49"/>
       <c r="G45" s="49"/>
       <c r="H45" s="50" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="I45" s="52" t="n">
         <f aca="false">COUNTIF(I8:I42,"Fail")</f>
@@ -3213,13 +3223,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4372469635628"/>
@@ -3256,7 +3266,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -3274,7 +3284,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -3289,10 +3299,10 @@
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -3307,10 +3317,10 @@
     </row>
     <row r="5" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="34" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
@@ -3343,31 +3353,31 @@
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="J7" s="30"/>
     </row>
@@ -3376,14 +3386,14 @@
         <v>1</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C8" s="37"/>
       <c r="D8" s="38" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F8" s="40"/>
       <c r="G8" s="41"/>
@@ -3396,14 +3406,14 @@
         <v>2</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C9" s="37"/>
       <c r="D9" s="38" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E9" s="39" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F9" s="44"/>
       <c r="G9" s="45"/>
@@ -3416,18 +3426,18 @@
         <v>3</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="38" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E10" s="39" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F10" s="44"/>
       <c r="G10" s="45" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H10" s="42"/>
       <c r="I10" s="43"/>
@@ -3438,14 +3448,14 @@
         <v>4</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C11" s="37"/>
       <c r="D11" s="38" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E11" s="39" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F11" s="44"/>
       <c r="G11" s="45"/>
@@ -3458,18 +3468,18 @@
         <v>5</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C12" s="37"/>
       <c r="D12" s="38" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E12" s="39"/>
       <c r="F12" s="40" t="n">
         <v>1</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H12" s="42"/>
       <c r="I12" s="43"/>
@@ -3480,15 +3490,15 @@
         <v>6</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C13" s="37"/>
       <c r="D13" s="38" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="44" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="G13" s="45"/>
       <c r="H13" s="42"/>
@@ -3500,14 +3510,14 @@
         <v>7</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="38" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F14" s="44"/>
       <c r="G14" s="45"/>
@@ -3541,7 +3551,7 @@
       <c r="F16" s="49"/>
       <c r="G16" s="49"/>
       <c r="H16" s="50" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="I16" s="51" t="n">
         <f aca="false">COUNTIF(I8:I14,"Pass")</f>
@@ -3558,7 +3568,7 @@
       <c r="F17" s="49"/>
       <c r="G17" s="49"/>
       <c r="H17" s="50" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="I17" s="52" t="n">
         <f aca="false">COUNTIF(I8:I14,"Fail")</f>
@@ -3566,7 +3576,6 @@
       </c>
       <c r="J17" s="30"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B1:G1"/>

</xml_diff>